<commit_message>
Few More Pages added
</commit_message>
<xml_diff>
--- a/data/sitTestData.xlsx
+++ b/data/sitTestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/animeshkoley/Projects/GitHub/orangehrm-playwright-js-framework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A0CEE8-4D19-9947-AED7-5B677B1B512A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F4BF03-51F9-F849-9C47-07066FE52B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{005DFED5-BBD0-8E4D-831B-E274BC7F678E}"/>
+    <workbookView xWindow="6880" yWindow="24560" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{005DFED5-BBD0-8E4D-831B-E274BC7F678E}"/>
   </bookViews>
   <sheets>
     <sheet name="url" sheetId="1" r:id="rId1"/>
+    <sheet name="addSingleUser" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>loginPage</t>
   </si>
@@ -54,6 +55,33 @@
   </si>
   <si>
     <t>URL Path</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>tin01ak</t>
+  </si>
+  <si>
+    <t>re5tr1ct$</t>
+  </si>
+  <si>
+    <t>userRole</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>newUsername</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>tin02ak</t>
   </si>
 </sst>
 </file>
@@ -427,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5867896-BDC8-754E-8099-88377F3CEC21}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -464,4 +492,66 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2FCEEF5-D204-3A47-807A-BF6FD3E0DE1D}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added a test to check the datePicker utility created by me
</commit_message>
<xml_diff>
--- a/data/sitTestData.xlsx
+++ b/data/sitTestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/animeshkoley/Projects/GitHub/orangehrm-playwright-js-framework/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F4BF03-51F9-F849-9C47-07066FE52B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B04FE48A-2703-5340-8AF4-932E6069A130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6880" yWindow="24560" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{005DFED5-BBD0-8E4D-831B-E274BC7F678E}"/>
+    <workbookView xWindow="6880" yWindow="24560" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{005DFED5-BBD0-8E4D-831B-E274BC7F678E}"/>
   </bookViews>
   <sheets>
     <sheet name="url" sheetId="1" r:id="rId1"/>
     <sheet name="addSingleUser" sheetId="2" r:id="rId2"/>
+    <sheet name="myInfoDate" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>loginPage</t>
   </si>
@@ -82,6 +83,9 @@
   </si>
   <si>
     <t>tin02ak</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -498,7 +502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2FCEEF5-D204-3A47-807A-BF6FD3E0DE1D}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -554,4 +558,27 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F1A9A2-7E7E-354A-9169-6FDF815EA507}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1">
+        <v>19900409</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>